<commit_message>
Update comments, excel sheets
</commit_message>
<xml_diff>
--- a/results/CrewMemberDeath.xlsx
+++ b/results/CrewMemberDeath.xlsx
@@ -255,25 +255,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>7.3749999999999902</c:v>
+                  <c:v>7.2666666666666604</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.8615384615383999</c:v>
+                  <c:v>6.9428571428571404</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.2349999999999994</c:v>
+                  <c:v>7.0124999999999904</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.140625</c:v>
+                  <c:v>6.3388888888888797</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.6864864864864799</c:v>
+                  <c:v>6.5444444444444398</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.7631578947368398</c:v>
+                  <c:v>6.4666666666666597</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.9175675675675601</c:v>
+                  <c:v>6.6099999999999897</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -344,25 +344,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.649519052838328</c:v>
+                  <c:v>0.68960536218590596</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.27919168264445</c:v>
+                  <c:v>0.48360888228030702</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5758410452834299</c:v>
+                  <c:v>0.45672064766112702</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.67254659408191</c:v>
+                  <c:v>1.3338077859558799</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2156995899730401</c:v>
+                  <c:v>1.1535238549551601</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5728654796817501</c:v>
+                  <c:v>1.55313303429623</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.54332548178662</c:v>
+                  <c:v>1.1707594875881899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -433,25 +433,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>6.5684467918622804</c:v>
+                  <c:v>6.5565029348161801</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.4085344827586104</c:v>
+                  <c:v>6.4186928104575101</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.4395272292040504</c:v>
+                  <c:v>6.4297417631344498</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.3615757575757499</c:v>
+                  <c:v>6.1940327237728496</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.3781151832460701</c:v>
+                  <c:v>6.2612708018154297</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.5795620437956099</c:v>
+                  <c:v>6.5571428571428498</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.3639152102196901</c:v>
+                  <c:v>6.4970846306255599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -522,25 +522,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.25659609174118</c:v>
+                  <c:v>1.1476770824495399</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.26003575093667</c:v>
+                  <c:v>1.2155838279976701</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.31702796969424</c:v>
+                  <c:v>1.2958790169746499</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4390872323951001</c:v>
+                  <c:v>1.3940071801028899</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3723952414573199</c:v>
+                  <c:v>1.3128876677111201</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4827050976962699</c:v>
+                  <c:v>1.5362291495737199</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.21563331563451</c:v>
+                  <c:v>1.14754688229681</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1784,7 +1784,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1818,16 +1818,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>7.3749999999999902</v>
+        <v>7.2666666666666604</v>
       </c>
       <c r="C2">
-        <v>0.649519052838328</v>
+        <v>0.68960536218590596</v>
       </c>
       <c r="D2">
-        <v>6.5684467918622804</v>
+        <v>6.5565029348161801</v>
       </c>
       <c r="E2">
-        <v>1.25659609174118</v>
+        <v>1.1476770824495399</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1835,16 +1835,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>6.8615384615383999</v>
+        <v>6.9428571428571404</v>
       </c>
       <c r="C3">
-        <v>1.27919168264445</v>
+        <v>0.48360888228030702</v>
       </c>
       <c r="D3">
-        <v>6.4085344827586104</v>
+        <v>6.4186928104575101</v>
       </c>
       <c r="E3">
-        <v>1.26003575093667</v>
+        <v>1.2155838279976701</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1852,16 +1852,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>8.2349999999999994</v>
+        <v>7.0124999999999904</v>
       </c>
       <c r="C4">
-        <v>1.5758410452834299</v>
+        <v>0.45672064766112702</v>
       </c>
       <c r="D4">
-        <v>6.4395272292040504</v>
+        <v>6.4297417631344498</v>
       </c>
       <c r="E4">
-        <v>1.31702796969424</v>
+        <v>1.2958790169746499</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1869,16 +1869,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>6.140625</v>
+        <v>6.3388888888888797</v>
       </c>
       <c r="C5">
-        <v>1.67254659408191</v>
+        <v>1.3338077859558799</v>
       </c>
       <c r="D5">
-        <v>6.3615757575757499</v>
+        <v>6.1940327237728496</v>
       </c>
       <c r="E5">
-        <v>1.4390872323951001</v>
+        <v>1.3940071801028899</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1886,16 +1886,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>6.6864864864864799</v>
+        <v>6.5444444444444398</v>
       </c>
       <c r="C6">
-        <v>1.2156995899730401</v>
+        <v>1.1535238549551601</v>
       </c>
       <c r="D6">
-        <v>6.3781151832460701</v>
+        <v>6.2612708018154297</v>
       </c>
       <c r="E6">
-        <v>1.3723952414573199</v>
+        <v>1.3128876677111201</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1903,16 +1903,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>6.7631578947368398</v>
+        <v>6.4666666666666597</v>
       </c>
       <c r="C7">
-        <v>1.5728654796817501</v>
+        <v>1.55313303429623</v>
       </c>
       <c r="D7">
-        <v>6.5795620437956099</v>
+        <v>6.5571428571428498</v>
       </c>
       <c r="E7">
-        <v>1.4827050976962699</v>
+        <v>1.5362291495737199</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1920,16 +1920,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>6.9175675675675601</v>
+        <v>6.6099999999999897</v>
       </c>
       <c r="C8">
-        <v>1.54332548178662</v>
+        <v>1.1707594875881899</v>
       </c>
       <c r="D8">
-        <v>6.3639152102196901</v>
+        <v>6.4970846306255599</v>
       </c>
       <c r="E8">
-        <v>1.21563331563451</v>
+        <v>1.14754688229681</v>
       </c>
     </row>
   </sheetData>

</xml_diff>